<commit_message>
Almost finished creating tables for the AI Programming report. Need to get the averages of the values to show the best environment for the AI to perform in. Also need to fix design flaw preveting Tallon from seeing obstacles adjacently in front of it due to only seeing the obstacle closest to its grid value location
</commit_message>
<xml_diff>
--- a/Advanced Artificial Intelligence/AAI Assignment 2/Advanced Artificial Intelligence Assignment 2 report grids.xlsx
+++ b/Advanced Artificial Intelligence/AAI Assignment 2/Advanced Artificial Intelligence Assignment 2 report grids.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff494b0457865fe3/Desktop/MSc-Robotics-and-Autonomous-Systems/Advanced Artificial Intelligence/AAI Assignment 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghost_000\Desktop\MSc-Robotics-and-Autonomous-Systems\Advanced Artificial Intelligence\AAI Assignment 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="222" documentId="8_{73268A56-61C3-4C1C-8493-C2CAE312CB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B038C2F4-F3E7-4CC4-BECB-E553E1E1937F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C2BF46-DAEB-4060-813A-A30FE15BB21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{1815FF3B-F9B4-4C41-88AE-2F0F6C802314}"/>
+    <workbookView xWindow="5115" yWindow="1935" windowWidth="15375" windowHeight="7875" xr2:uid="{1815FF3B-F9B4-4C41-88AE-2F0F6C802314}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -793,74 +793,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{706704AF-AAF0-45DC-95A8-849BFB62573A}">
   <dimension ref="A2:AC52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="X32" sqref="X32"/>
+    <sheetView tabSelected="1" topLeftCell="V16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AC28" sqref="AC28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="8.7265625" customWidth="1"/>
-    <col min="4" max="4" width="6.1796875" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" customWidth="1"/>
-    <col min="17" max="17" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.453125" customWidth="1"/>
-    <col min="24" max="24" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.81640625" customWidth="1"/>
-    <col min="29" max="29" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.42578125" customWidth="1"/>
+    <col min="24" max="24" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.85546875" customWidth="1"/>
+    <col min="29" max="29" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -879,8 +879,11 @@
       <c r="Z12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AB12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -911,8 +914,11 @@
       <c r="Z13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AB13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -943,8 +949,11 @@
       <c r="Z14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="AB14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -979,7 +988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -996,7 +1005,7 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1024,7 +1033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1096,7 +1105,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1161,11 +1170,17 @@
       <c r="Z19" s="34">
         <v>1</v>
       </c>
-      <c r="AA19" s="7"/>
-      <c r="AB19" s="28"/>
-      <c r="AC19" s="29"/>
-    </row>
-    <row r="20" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AA19" s="7">
+        <v>3</v>
+      </c>
+      <c r="AB19" s="28">
+        <v>11</v>
+      </c>
+      <c r="AC19" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1230,11 +1245,17 @@
       <c r="Z20" s="35">
         <v>2</v>
       </c>
-      <c r="AA20" s="26"/>
-      <c r="AB20" s="3"/>
-      <c r="AC20" s="4"/>
-    </row>
-    <row r="21" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AA20" s="26">
+        <v>5</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>22</v>
+      </c>
+      <c r="AC20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1299,11 +1320,17 @@
       <c r="Z21" s="35">
         <v>3</v>
       </c>
-      <c r="AA21" s="26"/>
-      <c r="AB21" s="3"/>
-      <c r="AC21" s="4"/>
-    </row>
-    <row r="22" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AA21" s="26">
+        <v>65</v>
+      </c>
+      <c r="AB21" s="3">
+        <v>52</v>
+      </c>
+      <c r="AC21" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1368,11 +1395,17 @@
       <c r="Z22" s="35">
         <v>4</v>
       </c>
-      <c r="AA22" s="26"/>
-      <c r="AB22" s="3"/>
-      <c r="AC22" s="4"/>
-    </row>
-    <row r="23" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AA22" s="26">
+        <v>2</v>
+      </c>
+      <c r="AB22" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1437,11 +1470,17 @@
       <c r="Z23" s="35">
         <v>5</v>
       </c>
-      <c r="AA23" s="26"/>
-      <c r="AB23" s="3"/>
-      <c r="AC23" s="4"/>
-    </row>
-    <row r="24" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AA23" s="26">
+        <v>5</v>
+      </c>
+      <c r="AB23" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC23" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
@@ -1508,11 +1547,17 @@
       <c r="Z24" s="35">
         <v>6</v>
       </c>
-      <c r="AA24" s="26"/>
-      <c r="AB24" s="3"/>
-      <c r="AC24" s="4"/>
-    </row>
-    <row r="25" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AA24" s="26">
+        <v>28</v>
+      </c>
+      <c r="AB24" s="3">
+        <v>24</v>
+      </c>
+      <c r="AC24" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1577,11 +1622,17 @@
       <c r="Z25" s="35">
         <v>7</v>
       </c>
-      <c r="AA25" s="26"/>
-      <c r="AB25" s="3"/>
-      <c r="AC25" s="4"/>
-    </row>
-    <row r="26" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AA25" s="26">
+        <v>16</v>
+      </c>
+      <c r="AB25" s="3">
+        <v>8</v>
+      </c>
+      <c r="AC25" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1646,11 +1697,17 @@
       <c r="Z26" s="35">
         <v>8</v>
       </c>
-      <c r="AA26" s="26"/>
-      <c r="AB26" s="3"/>
-      <c r="AC26" s="4"/>
-    </row>
-    <row r="27" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AA26" s="26">
+        <v>5</v>
+      </c>
+      <c r="AB26" s="3">
+        <v>32</v>
+      </c>
+      <c r="AC26" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1715,11 +1772,17 @@
       <c r="Z27" s="35">
         <v>9</v>
       </c>
-      <c r="AA27" s="26"/>
-      <c r="AB27" s="3"/>
-      <c r="AC27" s="4"/>
-    </row>
-    <row r="28" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AA27" s="26">
+        <v>5</v>
+      </c>
+      <c r="AB27" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1784,11 +1847,17 @@
       <c r="Z28" s="36">
         <v>10</v>
       </c>
-      <c r="AA28" s="27"/>
-      <c r="AB28" s="5"/>
-      <c r="AC28" s="6"/>
-    </row>
-    <row r="29" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AA28" s="27">
+        <v>9</v>
+      </c>
+      <c r="AB28" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC28" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1811,7 +1880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P30" s="30" t="s">
         <v>1</v>
       </c>
@@ -1849,7 +1918,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="P31" s="34">
         <v>1</v>
       </c>
@@ -1881,7 +1950,7 @@
       <c r="AB31" s="28"/>
       <c r="AC31" s="29"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="P32" s="35">
         <v>2</v>
       </c>
@@ -1897,9 +1966,15 @@
       <c r="U32" s="35">
         <v>2</v>
       </c>
-      <c r="V32" s="26"/>
-      <c r="W32" s="3"/>
-      <c r="X32" s="4"/>
+      <c r="V32" s="26">
+        <v>1</v>
+      </c>
+      <c r="W32" s="3">
+        <v>10</v>
+      </c>
+      <c r="X32" s="4">
+        <v>1</v>
+      </c>
       <c r="Z32" s="35">
         <v>2</v>
       </c>
@@ -1907,7 +1982,7 @@
       <c r="AB32" s="3"/>
       <c r="AC32" s="4"/>
     </row>
-    <row r="33" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="33" spans="16:29" x14ac:dyDescent="0.25">
       <c r="P33" s="35">
         <v>3</v>
       </c>
@@ -1923,9 +1998,15 @@
       <c r="U33" s="35">
         <v>3</v>
       </c>
-      <c r="V33" s="26"/>
-      <c r="W33" s="3"/>
-      <c r="X33" s="4"/>
+      <c r="V33" s="26">
+        <v>2</v>
+      </c>
+      <c r="W33" s="3">
+        <v>21</v>
+      </c>
+      <c r="X33" s="4">
+        <v>1</v>
+      </c>
       <c r="Z33" s="35">
         <v>3</v>
       </c>
@@ -1933,7 +2014,7 @@
       <c r="AB33" s="3"/>
       <c r="AC33" s="4"/>
     </row>
-    <row r="34" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="34" spans="16:29" x14ac:dyDescent="0.25">
       <c r="P34" s="35">
         <v>4</v>
       </c>
@@ -1949,9 +2030,15 @@
       <c r="U34" s="35">
         <v>4</v>
       </c>
-      <c r="V34" s="26"/>
-      <c r="W34" s="3"/>
-      <c r="X34" s="4"/>
+      <c r="V34" s="26">
+        <v>1</v>
+      </c>
+      <c r="W34" s="3">
+        <v>0</v>
+      </c>
+      <c r="X34" s="4">
+        <v>1</v>
+      </c>
       <c r="Z34" s="35">
         <v>4</v>
       </c>
@@ -1959,7 +2046,7 @@
       <c r="AB34" s="3"/>
       <c r="AC34" s="4"/>
     </row>
-    <row r="35" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="35" spans="16:29" x14ac:dyDescent="0.25">
       <c r="P35" s="35">
         <v>5</v>
       </c>
@@ -1975,9 +2062,15 @@
       <c r="U35" s="35">
         <v>5</v>
       </c>
-      <c r="V35" s="26"/>
-      <c r="W35" s="3"/>
-      <c r="X35" s="4"/>
+      <c r="V35" s="26">
+        <v>3</v>
+      </c>
+      <c r="W35" s="3">
+        <v>11</v>
+      </c>
+      <c r="X35" s="4">
+        <v>1</v>
+      </c>
       <c r="Z35" s="35">
         <v>5</v>
       </c>
@@ -1985,7 +2078,7 @@
       <c r="AB35" s="3"/>
       <c r="AC35" s="4"/>
     </row>
-    <row r="36" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="36" spans="16:29" x14ac:dyDescent="0.25">
       <c r="P36" s="35">
         <v>6</v>
       </c>
@@ -2001,9 +2094,15 @@
       <c r="U36" s="35">
         <v>6</v>
       </c>
-      <c r="V36" s="26"/>
-      <c r="W36" s="3"/>
-      <c r="X36" s="4"/>
+      <c r="V36" s="26">
+        <v>1</v>
+      </c>
+      <c r="W36" s="3">
+        <v>0</v>
+      </c>
+      <c r="X36" s="4">
+        <v>1</v>
+      </c>
       <c r="Z36" s="35">
         <v>6</v>
       </c>
@@ -2011,7 +2110,7 @@
       <c r="AB36" s="3"/>
       <c r="AC36" s="4"/>
     </row>
-    <row r="37" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="37" spans="16:29" x14ac:dyDescent="0.25">
       <c r="P37" s="35">
         <v>7</v>
       </c>
@@ -2027,9 +2126,15 @@
       <c r="U37" s="35">
         <v>7</v>
       </c>
-      <c r="V37" s="26"/>
-      <c r="W37" s="3"/>
-      <c r="X37" s="4"/>
+      <c r="V37" s="26">
+        <v>1</v>
+      </c>
+      <c r="W37" s="3">
+        <v>0</v>
+      </c>
+      <c r="X37" s="4">
+        <v>1</v>
+      </c>
       <c r="Z37" s="35">
         <v>7</v>
       </c>
@@ -2037,7 +2142,7 @@
       <c r="AB37" s="3"/>
       <c r="AC37" s="4"/>
     </row>
-    <row r="38" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="38" spans="16:29" x14ac:dyDescent="0.25">
       <c r="P38" s="35">
         <v>8</v>
       </c>
@@ -2053,9 +2158,15 @@
       <c r="U38" s="35">
         <v>8</v>
       </c>
-      <c r="V38" s="26"/>
-      <c r="W38" s="3"/>
-      <c r="X38" s="4"/>
+      <c r="V38" s="26">
+        <v>1</v>
+      </c>
+      <c r="W38" s="3">
+        <v>0</v>
+      </c>
+      <c r="X38" s="4">
+        <v>1</v>
+      </c>
       <c r="Z38" s="35">
         <v>8</v>
       </c>
@@ -2063,7 +2174,7 @@
       <c r="AB38" s="3"/>
       <c r="AC38" s="4"/>
     </row>
-    <row r="39" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="39" spans="16:29" x14ac:dyDescent="0.25">
       <c r="P39" s="35">
         <v>9</v>
       </c>
@@ -2079,9 +2190,15 @@
       <c r="U39" s="35">
         <v>9</v>
       </c>
-      <c r="V39" s="26"/>
-      <c r="W39" s="3"/>
-      <c r="X39" s="4"/>
+      <c r="V39" s="26">
+        <v>2</v>
+      </c>
+      <c r="W39" s="3">
+        <v>1</v>
+      </c>
+      <c r="X39" s="4">
+        <v>1</v>
+      </c>
       <c r="Z39" s="35">
         <v>9</v>
       </c>
@@ -2089,7 +2206,7 @@
       <c r="AB39" s="3"/>
       <c r="AC39" s="4"/>
     </row>
-    <row r="40" spans="16:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="16:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P40" s="36">
         <v>10</v>
       </c>
@@ -2105,9 +2222,15 @@
       <c r="U40" s="36">
         <v>10</v>
       </c>
-      <c r="V40" s="27"/>
-      <c r="W40" s="5"/>
-      <c r="X40" s="6"/>
+      <c r="V40" s="27">
+        <v>4</v>
+      </c>
+      <c r="W40" s="5">
+        <v>22</v>
+      </c>
+      <c r="X40" s="6">
+        <v>1</v>
+      </c>
       <c r="Z40" s="36">
         <v>10</v>
       </c>
@@ -2115,7 +2238,7 @@
       <c r="AB40" s="5"/>
       <c r="AC40" s="6"/>
     </row>
-    <row r="41" spans="16:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="16:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P41" t="s">
         <v>10</v>
       </c>
@@ -2126,7 +2249,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="16:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="16:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P42" s="30" t="s">
         <v>1</v>
       </c>
@@ -2164,7 +2287,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="43" spans="16:29" x14ac:dyDescent="0.25">
       <c r="P43" s="34">
         <v>1</v>
       </c>
@@ -2180,9 +2303,15 @@
       <c r="U43" s="34">
         <v>1</v>
       </c>
-      <c r="V43" s="7"/>
-      <c r="W43" s="28"/>
-      <c r="X43" s="29"/>
+      <c r="V43" s="7">
+        <v>7</v>
+      </c>
+      <c r="W43" s="28">
+        <v>3</v>
+      </c>
+      <c r="X43" s="29">
+        <v>0</v>
+      </c>
       <c r="Z43" s="34">
         <v>1</v>
       </c>
@@ -2190,7 +2319,7 @@
       <c r="AB43" s="28"/>
       <c r="AC43" s="29"/>
     </row>
-    <row r="44" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="44" spans="16:29" x14ac:dyDescent="0.25">
       <c r="P44" s="35">
         <v>2</v>
       </c>
@@ -2206,9 +2335,15 @@
       <c r="U44" s="35">
         <v>2</v>
       </c>
-      <c r="V44" s="26"/>
-      <c r="W44" s="3"/>
-      <c r="X44" s="4"/>
+      <c r="V44" s="26">
+        <v>15</v>
+      </c>
+      <c r="W44" s="3">
+        <v>17</v>
+      </c>
+      <c r="X44" s="4">
+        <v>1</v>
+      </c>
       <c r="Z44" s="35">
         <v>2</v>
       </c>
@@ -2216,7 +2351,7 @@
       <c r="AB44" s="3"/>
       <c r="AC44" s="4"/>
     </row>
-    <row r="45" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="45" spans="16:29" x14ac:dyDescent="0.25">
       <c r="P45" s="35">
         <v>3</v>
       </c>
@@ -2232,9 +2367,15 @@
       <c r="U45" s="35">
         <v>3</v>
       </c>
-      <c r="V45" s="26"/>
-      <c r="W45" s="3"/>
-      <c r="X45" s="4"/>
+      <c r="V45" s="26">
+        <v>32</v>
+      </c>
+      <c r="W45" s="3">
+        <v>16</v>
+      </c>
+      <c r="X45" s="4">
+        <v>1</v>
+      </c>
       <c r="Z45" s="35">
         <v>3</v>
       </c>
@@ -2242,7 +2383,7 @@
       <c r="AB45" s="3"/>
       <c r="AC45" s="4"/>
     </row>
-    <row r="46" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="46" spans="16:29" x14ac:dyDescent="0.25">
       <c r="P46" s="35">
         <v>4</v>
       </c>
@@ -2258,9 +2399,15 @@
       <c r="U46" s="35">
         <v>4</v>
       </c>
-      <c r="V46" s="26"/>
-      <c r="W46" s="3"/>
-      <c r="X46" s="4"/>
+      <c r="V46" s="26">
+        <v>6</v>
+      </c>
+      <c r="W46" s="3">
+        <v>3</v>
+      </c>
+      <c r="X46" s="4">
+        <v>1</v>
+      </c>
       <c r="Z46" s="35">
         <v>4</v>
       </c>
@@ -2268,7 +2415,7 @@
       <c r="AB46" s="3"/>
       <c r="AC46" s="4"/>
     </row>
-    <row r="47" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="47" spans="16:29" x14ac:dyDescent="0.25">
       <c r="P47" s="35">
         <v>5</v>
       </c>
@@ -2284,9 +2431,15 @@
       <c r="U47" s="35">
         <v>5</v>
       </c>
-      <c r="V47" s="26"/>
-      <c r="W47" s="3"/>
-      <c r="X47" s="4"/>
+      <c r="V47" s="26">
+        <v>11</v>
+      </c>
+      <c r="W47" s="3">
+        <v>5</v>
+      </c>
+      <c r="X47" s="4">
+        <v>2</v>
+      </c>
       <c r="Z47" s="35">
         <v>5</v>
       </c>
@@ -2294,7 +2447,7 @@
       <c r="AB47" s="3"/>
       <c r="AC47" s="4"/>
     </row>
-    <row r="48" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="48" spans="16:29" x14ac:dyDescent="0.25">
       <c r="P48" s="35">
         <v>6</v>
       </c>
@@ -2310,9 +2463,15 @@
       <c r="U48" s="35">
         <v>6</v>
       </c>
-      <c r="V48" s="26"/>
-      <c r="W48" s="3"/>
-      <c r="X48" s="4"/>
+      <c r="V48" s="26">
+        <v>19</v>
+      </c>
+      <c r="W48" s="3">
+        <v>9</v>
+      </c>
+      <c r="X48" s="4">
+        <v>1</v>
+      </c>
       <c r="Z48" s="35">
         <v>6</v>
       </c>
@@ -2320,7 +2479,7 @@
       <c r="AB48" s="3"/>
       <c r="AC48" s="4"/>
     </row>
-    <row r="49" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="49" spans="16:29" x14ac:dyDescent="0.25">
       <c r="P49" s="35">
         <v>7</v>
       </c>
@@ -2336,9 +2495,15 @@
       <c r="U49" s="35">
         <v>7</v>
       </c>
-      <c r="V49" s="26"/>
-      <c r="W49" s="3"/>
-      <c r="X49" s="4"/>
+      <c r="V49" s="26">
+        <v>26</v>
+      </c>
+      <c r="W49" s="3">
+        <v>13</v>
+      </c>
+      <c r="X49" s="4">
+        <v>1</v>
+      </c>
       <c r="Z49" s="35">
         <v>7</v>
       </c>
@@ -2346,7 +2511,7 @@
       <c r="AB49" s="3"/>
       <c r="AC49" s="4"/>
     </row>
-    <row r="50" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="50" spans="16:29" x14ac:dyDescent="0.25">
       <c r="P50" s="35">
         <v>8</v>
       </c>
@@ -2362,9 +2527,15 @@
       <c r="U50" s="35">
         <v>8</v>
       </c>
-      <c r="V50" s="26"/>
-      <c r="W50" s="3"/>
-      <c r="X50" s="4"/>
+      <c r="V50" s="26">
+        <v>163</v>
+      </c>
+      <c r="W50" s="3">
+        <v>91</v>
+      </c>
+      <c r="X50" s="4">
+        <v>2</v>
+      </c>
       <c r="Z50" s="35">
         <v>8</v>
       </c>
@@ -2372,7 +2543,7 @@
       <c r="AB50" s="3"/>
       <c r="AC50" s="4"/>
     </row>
-    <row r="51" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="51" spans="16:29" x14ac:dyDescent="0.25">
       <c r="P51" s="35">
         <v>9</v>
       </c>
@@ -2388,9 +2559,15 @@
       <c r="U51" s="35">
         <v>9</v>
       </c>
-      <c r="V51" s="26"/>
-      <c r="W51" s="3"/>
-      <c r="X51" s="4"/>
+      <c r="V51" s="26">
+        <v>112</v>
+      </c>
+      <c r="W51" s="3">
+        <v>56</v>
+      </c>
+      <c r="X51" s="4">
+        <v>1</v>
+      </c>
       <c r="Z51" s="35">
         <v>9</v>
       </c>
@@ -2398,7 +2575,7 @@
       <c r="AB51" s="3"/>
       <c r="AC51" s="4"/>
     </row>
-    <row r="52" spans="16:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="16:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P52" s="36">
         <v>10</v>
       </c>
@@ -2414,9 +2591,15 @@
       <c r="U52" s="36">
         <v>10</v>
       </c>
-      <c r="V52" s="27"/>
-      <c r="W52" s="5"/>
-      <c r="X52" s="6"/>
+      <c r="V52" s="27">
+        <v>11</v>
+      </c>
+      <c r="W52" s="5">
+        <v>5</v>
+      </c>
+      <c r="X52" s="6">
+        <v>2</v>
+      </c>
       <c r="Z52" s="36">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Almost finished all programming necessary for Advanced AI Assignment Report, Improved Tallon's navigation in a partially observable scenario so it can survive longer while avoiding obstacles and still collecting bonuses.
</commit_message>
<xml_diff>
--- a/Advanced Artificial Intelligence/AAI Assignment 2/Advanced Artificial Intelligence Assignment 2 report grids.xlsx
+++ b/Advanced Artificial Intelligence/AAI Assignment 2/Advanced Artificial Intelligence Assignment 2 report grids.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghost_000\Desktop\MSc-Robotics-and-Autonomous-Systems\Advanced Artificial Intelligence\AAI Assignment 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff494b0457865fe3/Desktop/MSc-Robotics-and-Autonomous-Systems/Advanced Artificial Intelligence/AAI Assignment 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C2BF46-DAEB-4060-813A-A30FE15BB21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{68C2BF46-DAEB-4060-813A-A30FE15BB21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED24961E-DF6D-4FB0-B4B8-3E297E682742}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="1935" windowWidth="15375" windowHeight="7875" xr2:uid="{1815FF3B-F9B4-4C41-88AE-2F0F6C802314}"/>
+    <workbookView xWindow="2080" yWindow="2320" windowWidth="16540" windowHeight="8140" xr2:uid="{1815FF3B-F9B4-4C41-88AE-2F0F6C802314}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -793,74 +793,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{706704AF-AAF0-45DC-95A8-849BFB62573A}">
   <dimension ref="A2:AC52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC28" sqref="AC28"/>
+    <sheetView tabSelected="1" topLeftCell="P22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AC40" sqref="AC40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="17" max="17" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.42578125" customWidth="1"/>
-    <col min="24" max="24" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.85546875" customWidth="1"/>
-    <col min="29" max="29" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" customWidth="1"/>
+    <col min="4" max="4" width="6.1796875" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" customWidth="1"/>
+    <col min="17" max="17" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.453125" customWidth="1"/>
+    <col min="24" max="24" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.81640625" customWidth="1"/>
+    <col min="29" max="29" width="23.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -883,7 +883,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -918,7 +918,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -953,7 +953,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -988,7 +988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1005,7 +1005,7 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1033,7 +1033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1105,7 +1105,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1180,7 +1180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1255,7 +1255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1330,7 +1330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1405,7 +1405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1480,7 +1480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
@@ -1557,7 +1557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1632,7 +1632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1707,7 +1707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1782,7 +1782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1857,7 +1857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1877,10 +1877,10 @@
         <v>4</v>
       </c>
       <c r="Z29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="P30" s="30" t="s">
         <v>1</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.35">
       <c r="P31" s="34">
         <v>1</v>
       </c>
@@ -1946,11 +1946,17 @@
       <c r="Z31" s="34">
         <v>1</v>
       </c>
-      <c r="AA31" s="7"/>
-      <c r="AB31" s="28"/>
-      <c r="AC31" s="29"/>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AA31" s="7">
+        <v>5</v>
+      </c>
+      <c r="AB31" s="28">
+        <v>12</v>
+      </c>
+      <c r="AC31" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.35">
       <c r="P32" s="35">
         <v>2</v>
       </c>
@@ -1978,11 +1984,17 @@
       <c r="Z32" s="35">
         <v>2</v>
       </c>
-      <c r="AA32" s="26"/>
-      <c r="AB32" s="3"/>
-      <c r="AC32" s="4"/>
-    </row>
-    <row r="33" spans="16:29" x14ac:dyDescent="0.25">
+      <c r="AA32" s="26">
+        <v>2</v>
+      </c>
+      <c r="AB32" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC32" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="16:29" x14ac:dyDescent="0.35">
       <c r="P33" s="35">
         <v>3</v>
       </c>
@@ -2010,11 +2022,17 @@
       <c r="Z33" s="35">
         <v>3</v>
       </c>
-      <c r="AA33" s="26"/>
-      <c r="AB33" s="3"/>
-      <c r="AC33" s="4"/>
-    </row>
-    <row r="34" spans="16:29" x14ac:dyDescent="0.25">
+      <c r="AA33" s="26">
+        <v>59</v>
+      </c>
+      <c r="AB33" s="3">
+        <v>39</v>
+      </c>
+      <c r="AC33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="16:29" x14ac:dyDescent="0.35">
       <c r="P34" s="35">
         <v>4</v>
       </c>
@@ -2042,11 +2060,17 @@
       <c r="Z34" s="35">
         <v>4</v>
       </c>
-      <c r="AA34" s="26"/>
-      <c r="AB34" s="3"/>
-      <c r="AC34" s="4"/>
-    </row>
-    <row r="35" spans="16:29" x14ac:dyDescent="0.25">
+      <c r="AA34" s="26">
+        <v>12</v>
+      </c>
+      <c r="AB34" s="3">
+        <v>16</v>
+      </c>
+      <c r="AC34" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="16:29" x14ac:dyDescent="0.35">
       <c r="P35" s="35">
         <v>5</v>
       </c>
@@ -2074,11 +2098,17 @@
       <c r="Z35" s="35">
         <v>5</v>
       </c>
-      <c r="AA35" s="26"/>
-      <c r="AB35" s="3"/>
-      <c r="AC35" s="4"/>
-    </row>
-    <row r="36" spans="16:29" x14ac:dyDescent="0.25">
+      <c r="AA35" s="26">
+        <v>2</v>
+      </c>
+      <c r="AB35" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC35" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="16:29" x14ac:dyDescent="0.35">
       <c r="P36" s="35">
         <v>6</v>
       </c>
@@ -2106,11 +2136,17 @@
       <c r="Z36" s="35">
         <v>6</v>
       </c>
-      <c r="AA36" s="26"/>
-      <c r="AB36" s="3"/>
-      <c r="AC36" s="4"/>
-    </row>
-    <row r="37" spans="16:29" x14ac:dyDescent="0.25">
+      <c r="AA36" s="26">
+        <v>25</v>
+      </c>
+      <c r="AB36" s="3">
+        <v>22</v>
+      </c>
+      <c r="AC36" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="16:29" x14ac:dyDescent="0.35">
       <c r="P37" s="35">
         <v>7</v>
       </c>
@@ -2138,11 +2174,17 @@
       <c r="Z37" s="35">
         <v>7</v>
       </c>
-      <c r="AA37" s="26"/>
-      <c r="AB37" s="3"/>
-      <c r="AC37" s="4"/>
-    </row>
-    <row r="38" spans="16:29" x14ac:dyDescent="0.25">
+      <c r="AA37" s="26">
+        <v>14</v>
+      </c>
+      <c r="AB37" s="3">
+        <v>7</v>
+      </c>
+      <c r="AC37" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="16:29" x14ac:dyDescent="0.35">
       <c r="P38" s="35">
         <v>8</v>
       </c>
@@ -2170,11 +2212,17 @@
       <c r="Z38" s="35">
         <v>8</v>
       </c>
-      <c r="AA38" s="26"/>
-      <c r="AB38" s="3"/>
-      <c r="AC38" s="4"/>
-    </row>
-    <row r="39" spans="16:29" x14ac:dyDescent="0.25">
+      <c r="AA38" s="26">
+        <v>5</v>
+      </c>
+      <c r="AB38" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC38" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="16:29" x14ac:dyDescent="0.35">
       <c r="P39" s="35">
         <v>9</v>
       </c>
@@ -2202,11 +2250,17 @@
       <c r="Z39" s="35">
         <v>9</v>
       </c>
-      <c r="AA39" s="26"/>
-      <c r="AB39" s="3"/>
-      <c r="AC39" s="4"/>
-    </row>
-    <row r="40" spans="16:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA39" s="26">
+        <v>53</v>
+      </c>
+      <c r="AB39" s="3">
+        <v>46</v>
+      </c>
+      <c r="AC39" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="16:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="P40" s="36">
         <v>10</v>
       </c>
@@ -2234,11 +2288,17 @@
       <c r="Z40" s="36">
         <v>10</v>
       </c>
-      <c r="AA40" s="27"/>
-      <c r="AB40" s="5"/>
-      <c r="AC40" s="6"/>
-    </row>
-    <row r="41" spans="16:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA40" s="27">
+        <v>97</v>
+      </c>
+      <c r="AB40" s="5">
+        <v>58</v>
+      </c>
+      <c r="AC40" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="16:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="P41" t="s">
         <v>10</v>
       </c>
@@ -2246,10 +2306,10 @@
         <v>10</v>
       </c>
       <c r="Z41" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="16:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="16:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="P42" s="30" t="s">
         <v>1</v>
       </c>
@@ -2287,7 +2347,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="16:29" x14ac:dyDescent="0.25">
+    <row r="43" spans="16:29" x14ac:dyDescent="0.35">
       <c r="P43" s="34">
         <v>1</v>
       </c>
@@ -2319,7 +2379,7 @@
       <c r="AB43" s="28"/>
       <c r="AC43" s="29"/>
     </row>
-    <row r="44" spans="16:29" x14ac:dyDescent="0.25">
+    <row r="44" spans="16:29" x14ac:dyDescent="0.35">
       <c r="P44" s="35">
         <v>2</v>
       </c>
@@ -2351,7 +2411,7 @@
       <c r="AB44" s="3"/>
       <c r="AC44" s="4"/>
     </row>
-    <row r="45" spans="16:29" x14ac:dyDescent="0.25">
+    <row r="45" spans="16:29" x14ac:dyDescent="0.35">
       <c r="P45" s="35">
         <v>3</v>
       </c>
@@ -2383,7 +2443,7 @@
       <c r="AB45" s="3"/>
       <c r="AC45" s="4"/>
     </row>
-    <row r="46" spans="16:29" x14ac:dyDescent="0.25">
+    <row r="46" spans="16:29" x14ac:dyDescent="0.35">
       <c r="P46" s="35">
         <v>4</v>
       </c>
@@ -2415,7 +2475,7 @@
       <c r="AB46" s="3"/>
       <c r="AC46" s="4"/>
     </row>
-    <row r="47" spans="16:29" x14ac:dyDescent="0.25">
+    <row r="47" spans="16:29" x14ac:dyDescent="0.35">
       <c r="P47" s="35">
         <v>5</v>
       </c>
@@ -2447,7 +2507,7 @@
       <c r="AB47" s="3"/>
       <c r="AC47" s="4"/>
     </row>
-    <row r="48" spans="16:29" x14ac:dyDescent="0.25">
+    <row r="48" spans="16:29" x14ac:dyDescent="0.35">
       <c r="P48" s="35">
         <v>6</v>
       </c>
@@ -2479,7 +2539,7 @@
       <c r="AB48" s="3"/>
       <c r="AC48" s="4"/>
     </row>
-    <row r="49" spans="16:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="16:29" x14ac:dyDescent="0.35">
       <c r="P49" s="35">
         <v>7</v>
       </c>
@@ -2511,7 +2571,7 @@
       <c r="AB49" s="3"/>
       <c r="AC49" s="4"/>
     </row>
-    <row r="50" spans="16:29" x14ac:dyDescent="0.25">
+    <row r="50" spans="16:29" x14ac:dyDescent="0.35">
       <c r="P50" s="35">
         <v>8</v>
       </c>
@@ -2543,7 +2603,7 @@
       <c r="AB50" s="3"/>
       <c r="AC50" s="4"/>
     </row>
-    <row r="51" spans="16:29" x14ac:dyDescent="0.25">
+    <row r="51" spans="16:29" x14ac:dyDescent="0.35">
       <c r="P51" s="35">
         <v>9</v>
       </c>
@@ -2575,7 +2635,7 @@
       <c r="AB51" s="3"/>
       <c r="AC51" s="4"/>
     </row>
-    <row r="52" spans="16:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="16:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="P52" s="36">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Uploaded a copy of report and Assignment code. Need to improve the evaluation in the AAI report on the 14/02/2022 before submitting again
</commit_message>
<xml_diff>
--- a/Advanced Artificial Intelligence/AAI Assignment 2/Advanced Artificial Intelligence Assignment 2 report grids.xlsx
+++ b/Advanced Artificial Intelligence/AAI Assignment 2/Advanced Artificial Intelligence Assignment 2 report grids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff494b0457865fe3/Desktop/MSc-Robotics-and-Autonomous-Systems/Advanced Artificial Intelligence/AAI Assignment 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{68C2BF46-DAEB-4060-813A-A30FE15BB21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED24961E-DF6D-4FB0-B4B8-3E297E682742}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{68C2BF46-DAEB-4060-813A-A30FE15BB21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF997291-D89E-4707-903C-275323673D06}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="2320" windowWidth="16540" windowHeight="8140" xr2:uid="{1815FF3B-F9B4-4C41-88AE-2F0F6C802314}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{1815FF3B-F9B4-4C41-88AE-2F0F6C802314}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="15">
   <si>
     <t>State</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>number of Meanies in view</t>
+  </si>
+  <si>
+    <t>Scenario 1</t>
+  </si>
+  <si>
+    <t>Scenario 2</t>
+  </si>
+  <si>
+    <t>Scenario 3</t>
   </si>
 </sst>
 </file>
@@ -793,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{706704AF-AAF0-45DC-95A8-849BFB62573A}">
   <dimension ref="A2:AC52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC40" sqref="AC40"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -859,6 +868,15 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
+      <c r="P11" t="s">
+        <v>12</v>
+      </c>
+      <c r="U11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="M12" s="1"/>

</xml_diff>

<commit_message>
Finished all programming for AAI Assingment now, just improving report layout and will upload for the last time
</commit_message>
<xml_diff>
--- a/Advanced Artificial Intelligence/AAI Assignment 2/Advanced Artificial Intelligence Assignment 2 report grids.xlsx
+++ b/Advanced Artificial Intelligence/AAI Assignment 2/Advanced Artificial Intelligence Assignment 2 report grids.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff494b0457865fe3/Desktop/MSc-Robotics-and-Autonomous-Systems/Advanced Artificial Intelligence/AAI Assignment 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{68C2BF46-DAEB-4060-813A-A30FE15BB21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF997291-D89E-4707-903C-275323673D06}"/>
+  <xr:revisionPtr revIDLastSave="436" documentId="13_ncr:1_{68C2BF46-DAEB-4060-813A-A30FE15BB21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52B59186-EFA1-408D-8A68-46EDF857C54C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{1815FF3B-F9B4-4C41-88AE-2F0F6C802314}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="26">
   <si>
     <t>State</t>
   </si>
@@ -79,6 +79,39 @@
   </si>
   <si>
     <t>Scenario 3</t>
+  </si>
+  <si>
+    <t>10by10</t>
+  </si>
+  <si>
+    <t>5by5</t>
+  </si>
+  <si>
+    <t>15by15</t>
+  </si>
+  <si>
+    <t>scenario1</t>
+  </si>
+  <si>
+    <t>scenaio2</t>
+  </si>
+  <si>
+    <t>scenario3</t>
+  </si>
+  <si>
+    <t>average score</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Partial visibility set to TRUE</t>
+  </si>
+  <si>
+    <t>Partial visibility set to FALSE</t>
+  </si>
+  <si>
+    <t>average simulation time(seconds)</t>
   </si>
 </sst>
 </file>
@@ -132,7 +165,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -444,11 +477,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -486,6 +636,32 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,17 +976,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{706704AF-AAF0-45DC-95A8-849BFB62573A}">
-  <dimension ref="A2:AC52"/>
+  <dimension ref="A2:AC95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF19" sqref="AF19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="8.7265625" customWidth="1"/>
     <col min="4" max="4" width="6.1796875" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" customWidth="1"/>
+    <col min="5" max="6" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.453125" customWidth="1"/>
     <col min="17" max="17" width="19.54296875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="23.7265625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19.453125" customWidth="1"/>
@@ -2012,7 +2191,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="33" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G33" t="s">
+        <v>23</v>
+      </c>
       <c r="P33" s="35">
         <v>3</v>
       </c>
@@ -2050,7 +2232,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="34" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G34" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="47"/>
+      <c r="I34" s="47"/>
+      <c r="J34" s="47"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="48"/>
       <c r="P34" s="35">
         <v>4</v>
       </c>
@@ -2088,7 +2278,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="35" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G35" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="J35" s="47"/>
+      <c r="K35" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="L35" s="48"/>
       <c r="P35" s="35">
         <v>5</v>
       </c>
@@ -2126,7 +2328,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="36" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="G36" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="1">
+        <f>AVERAGE(R43:R52)</f>
+        <v>6.5</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="1">
+        <f>AVERAGE(W43:W52)</f>
+        <v>21.8</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="41">
+        <f>AVERAGE(AB31:AB40)</f>
+        <v>20.399999999999999</v>
+      </c>
       <c r="P36" s="35">
         <v>6</v>
       </c>
@@ -2164,7 +2387,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="37" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="G37" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="1">
+        <f>AVERAGE(R19:R28)</f>
+        <v>14.6</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J37" s="1">
+        <f>AVERAGE(W19:W28)</f>
+        <v>26.5</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L37" s="41">
+        <f>AVERAGE(AB19:AB28)</f>
+        <v>15.8</v>
+      </c>
       <c r="P37" s="35">
         <v>7</v>
       </c>
@@ -2202,7 +2446,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="38" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G38" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="43">
+        <f>AVERAGE(R31:R40)</f>
+        <v>5.3</v>
+      </c>
+      <c r="I38" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="43">
+        <f>AVERAGE(W31:W40)</f>
+        <v>6.5</v>
+      </c>
+      <c r="K38" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="L38" s="44" t="s">
+        <v>22</v>
+      </c>
       <c r="P38" s="35">
         <v>8</v>
       </c>
@@ -2240,7 +2504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="39" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="P39" s="35">
         <v>9</v>
       </c>
@@ -2278,7 +2542,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="16:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G40" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="H40" s="47"/>
+      <c r="I40" s="47"/>
+      <c r="J40" s="47"/>
+      <c r="K40" s="47"/>
+      <c r="L40" s="48"/>
       <c r="P40" s="36">
         <v>10</v>
       </c>
@@ -2316,7 +2588,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="16:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G41" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="H41" s="45"/>
+      <c r="I41" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="J41" s="45"/>
+      <c r="K41" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="L41" s="50"/>
       <c r="P41" t="s">
         <v>10</v>
       </c>
@@ -2327,7 +2611,28 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="16:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G42" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" s="38">
+        <f>AVERAGE(Q43:Q52)</f>
+        <v>13.4</v>
+      </c>
+      <c r="I42" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="38">
+        <f>AVERAGE(V43:V52)</f>
+        <v>40.200000000000003</v>
+      </c>
+      <c r="K42" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="L42" s="39">
+        <f>AVERAGE(AA31:AA40)</f>
+        <v>27.4</v>
+      </c>
       <c r="P42" s="30" t="s">
         <v>1</v>
       </c>
@@ -2365,7 +2670,28 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="43" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="G43" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" s="1">
+        <f>AVERAGE(Q19:Q28)</f>
+        <v>9.6</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J43" s="1">
+        <f>AVERAGE(V19:V28)</f>
+        <v>21.4</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L43" s="41">
+        <f>AVERAGE(AA19:AA28)</f>
+        <v>14.3</v>
+      </c>
       <c r="P43" s="34">
         <v>1</v>
       </c>
@@ -2397,7 +2723,27 @@
       <c r="AB43" s="28"/>
       <c r="AC43" s="29"/>
     </row>
-    <row r="44" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="44" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G44" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="43">
+        <f>AVERAGE(Q31:Q40)</f>
+        <v>3</v>
+      </c>
+      <c r="I44" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="J44" s="43">
+        <f>AVERAGE(V31:V40)</f>
+        <v>1.7</v>
+      </c>
+      <c r="K44" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="L44" s="44" t="s">
+        <v>22</v>
+      </c>
       <c r="P44" s="35">
         <v>2</v>
       </c>
@@ -2429,7 +2775,7 @@
       <c r="AB44" s="3"/>
       <c r="AC44" s="4"/>
     </row>
-    <row r="45" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="45" spans="7:29" x14ac:dyDescent="0.35">
       <c r="P45" s="35">
         <v>3</v>
       </c>
@@ -2461,7 +2807,7 @@
       <c r="AB45" s="3"/>
       <c r="AC45" s="4"/>
     </row>
-    <row r="46" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="46" spans="7:29" x14ac:dyDescent="0.35">
       <c r="P46" s="35">
         <v>4</v>
       </c>
@@ -2493,7 +2839,7 @@
       <c r="AB46" s="3"/>
       <c r="AC46" s="4"/>
     </row>
-    <row r="47" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="47" spans="7:29" x14ac:dyDescent="0.35">
       <c r="P47" s="35">
         <v>5</v>
       </c>
@@ -2525,7 +2871,7 @@
       <c r="AB47" s="3"/>
       <c r="AC47" s="4"/>
     </row>
-    <row r="48" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="48" spans="7:29" x14ac:dyDescent="0.35">
       <c r="P48" s="35">
         <v>6</v>
       </c>
@@ -2557,7 +2903,7 @@
       <c r="AB48" s="3"/>
       <c r="AC48" s="4"/>
     </row>
-    <row r="49" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="49" spans="7:29" x14ac:dyDescent="0.35">
       <c r="P49" s="35">
         <v>7</v>
       </c>
@@ -2589,7 +2935,7 @@
       <c r="AB49" s="3"/>
       <c r="AC49" s="4"/>
     </row>
-    <row r="50" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="50" spans="7:29" x14ac:dyDescent="0.35">
       <c r="P50" s="35">
         <v>8</v>
       </c>
@@ -2621,7 +2967,7 @@
       <c r="AB50" s="3"/>
       <c r="AC50" s="4"/>
     </row>
-    <row r="51" spans="16:29" x14ac:dyDescent="0.35">
+    <row r="51" spans="7:29" x14ac:dyDescent="0.35">
       <c r="P51" s="35">
         <v>9</v>
       </c>
@@ -2653,7 +2999,7 @@
       <c r="AB51" s="3"/>
       <c r="AC51" s="4"/>
     </row>
-    <row r="52" spans="16:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="P52" s="36">
         <v>10</v>
       </c>
@@ -2685,7 +3031,1510 @@
       <c r="AB52" s="5"/>
       <c r="AC52" s="6"/>
     </row>
+    <row r="54" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="P54" t="s">
+        <v>12</v>
+      </c>
+      <c r="U54" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="P55" t="s">
+        <v>7</v>
+      </c>
+      <c r="R55">
+        <v>5</v>
+      </c>
+      <c r="U55" t="s">
+        <v>7</v>
+      </c>
+      <c r="W55">
+        <v>10</v>
+      </c>
+      <c r="Z55" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB55">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="P56" t="s">
+        <v>6</v>
+      </c>
+      <c r="R56">
+        <v>3</v>
+      </c>
+      <c r="U56" t="s">
+        <v>6</v>
+      </c>
+      <c r="W56">
+        <v>6</v>
+      </c>
+      <c r="Z56" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB56">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="P57" t="s">
+        <v>5</v>
+      </c>
+      <c r="R57">
+        <v>3</v>
+      </c>
+      <c r="U57" t="s">
+        <v>5</v>
+      </c>
+      <c r="W57">
+        <v>6</v>
+      </c>
+      <c r="Z57" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB57">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="P58" t="s">
+        <v>9</v>
+      </c>
+      <c r="R58" t="b">
+        <v>0</v>
+      </c>
+      <c r="U58" t="s">
+        <v>9</v>
+      </c>
+      <c r="W58" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z58" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G60" t="s">
+        <v>24</v>
+      </c>
+      <c r="P60" t="s">
+        <v>3</v>
+      </c>
+      <c r="U60" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G61" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="H61" s="47"/>
+      <c r="I61" s="47"/>
+      <c r="J61" s="47"/>
+      <c r="K61" s="47"/>
+      <c r="L61" s="48"/>
+      <c r="P61" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q61" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="R61" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="S61" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="U61" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="V61" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="W61" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="X61" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z61" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA61" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB61" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC61" s="33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G62" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="H62" s="47"/>
+      <c r="I62" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="J62" s="47"/>
+      <c r="K62" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="L62" s="48"/>
+      <c r="P62" s="34">
+        <v>1</v>
+      </c>
+      <c r="Q62" s="7">
+        <v>4</v>
+      </c>
+      <c r="R62" s="28">
+        <v>12</v>
+      </c>
+      <c r="S62" s="29">
+        <v>2</v>
+      </c>
+      <c r="U62" s="34">
+        <v>1</v>
+      </c>
+      <c r="V62" s="7">
+        <v>2</v>
+      </c>
+      <c r="W62" s="28">
+        <v>5</v>
+      </c>
+      <c r="X62" s="29">
+        <v>1</v>
+      </c>
+      <c r="Z62" s="34">
+        <v>1</v>
+      </c>
+      <c r="AA62" s="7">
+        <v>2</v>
+      </c>
+      <c r="AB62" s="28">
+        <v>1</v>
+      </c>
+      <c r="AC62" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="G63" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="H63" s="1">
+        <f>AVERAGE(R86:R95)</f>
+        <v>13.7</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J63" s="1">
+        <f>AVERAGE(W86:W95)</f>
+        <v>23.5</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L63" s="41">
+        <f>AVERAGE(AB74:AB82)</f>
+        <v>9.2222222222222214</v>
+      </c>
+      <c r="P63" s="35">
+        <v>2</v>
+      </c>
+      <c r="Q63" s="26">
+        <v>15</v>
+      </c>
+      <c r="R63" s="3">
+        <v>17</v>
+      </c>
+      <c r="S63" s="4">
+        <v>3</v>
+      </c>
+      <c r="U63" s="35">
+        <v>2</v>
+      </c>
+      <c r="V63" s="26">
+        <v>13</v>
+      </c>
+      <c r="W63" s="3">
+        <v>26</v>
+      </c>
+      <c r="X63" s="4">
+        <v>2</v>
+      </c>
+      <c r="Z63" s="35">
+        <v>2</v>
+      </c>
+      <c r="AA63" s="26">
+        <v>26</v>
+      </c>
+      <c r="AB63" s="3">
+        <v>43</v>
+      </c>
+      <c r="AC63" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="G64" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H64" s="1">
+        <f>AVERAGE(R62:R71)</f>
+        <v>15.6</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J64" s="1">
+        <f>AVERAGE(W62:W71)</f>
+        <v>16.899999999999999</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L64" s="41">
+        <f>AVERAGE(AB62:AB70)</f>
+        <v>19.777777777777779</v>
+      </c>
+      <c r="P64" s="35">
+        <v>3</v>
+      </c>
+      <c r="Q64" s="26">
+        <v>4</v>
+      </c>
+      <c r="R64" s="3">
+        <v>2</v>
+      </c>
+      <c r="S64" s="4">
+        <v>2</v>
+      </c>
+      <c r="U64" s="35">
+        <v>3</v>
+      </c>
+      <c r="V64" s="26">
+        <v>7</v>
+      </c>
+      <c r="W64" s="3">
+        <v>3</v>
+      </c>
+      <c r="X64" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z64" s="35">
+        <v>3</v>
+      </c>
+      <c r="AA64" s="26">
+        <v>19</v>
+      </c>
+      <c r="AB64" s="3">
+        <v>29</v>
+      </c>
+      <c r="AC64" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G65" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="H65" s="43">
+        <f>AVERAGE(R74:R83)</f>
+        <v>10.1</v>
+      </c>
+      <c r="I65" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="J65" s="43">
+        <f>AVERAGE(W74:W82)</f>
+        <v>5.7777777777777777</v>
+      </c>
+      <c r="K65" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="L65" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="P65" s="35">
+        <v>4</v>
+      </c>
+      <c r="Q65" s="26">
+        <v>15</v>
+      </c>
+      <c r="R65" s="3">
+        <v>37</v>
+      </c>
+      <c r="S65" s="4">
+        <v>3</v>
+      </c>
+      <c r="U65" s="35">
+        <v>4</v>
+      </c>
+      <c r="V65" s="26">
+        <v>2</v>
+      </c>
+      <c r="W65" s="3">
+        <v>11</v>
+      </c>
+      <c r="X65" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z65" s="35">
+        <v>4</v>
+      </c>
+      <c r="AA65" s="26">
+        <v>15</v>
+      </c>
+      <c r="AB65" s="3">
+        <v>37</v>
+      </c>
+      <c r="AC65" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P66" s="35">
+        <v>5</v>
+      </c>
+      <c r="Q66" s="26">
+        <v>7</v>
+      </c>
+      <c r="R66" s="3">
+        <v>3</v>
+      </c>
+      <c r="S66" s="4">
+        <v>2</v>
+      </c>
+      <c r="U66" s="35">
+        <v>5</v>
+      </c>
+      <c r="V66" s="26">
+        <v>14</v>
+      </c>
+      <c r="W66" s="3">
+        <v>37</v>
+      </c>
+      <c r="X66" s="4">
+        <v>2</v>
+      </c>
+      <c r="Z66" s="35">
+        <v>5</v>
+      </c>
+      <c r="AA66" s="26">
+        <v>2</v>
+      </c>
+      <c r="AB66" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC66" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G67" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="H67" s="47"/>
+      <c r="I67" s="47"/>
+      <c r="J67" s="47"/>
+      <c r="K67" s="47"/>
+      <c r="L67" s="48"/>
+      <c r="P67" s="35">
+        <v>6</v>
+      </c>
+      <c r="Q67" s="26">
+        <v>6</v>
+      </c>
+      <c r="R67" s="3">
+        <v>13</v>
+      </c>
+      <c r="S67" s="4">
+        <v>2</v>
+      </c>
+      <c r="U67" s="35">
+        <v>6</v>
+      </c>
+      <c r="V67" s="26">
+        <v>11</v>
+      </c>
+      <c r="W67" s="3">
+        <v>15</v>
+      </c>
+      <c r="X67" s="4">
+        <v>2</v>
+      </c>
+      <c r="Z67" s="35">
+        <v>6</v>
+      </c>
+      <c r="AA67" s="26">
+        <v>10</v>
+      </c>
+      <c r="AB67" s="3">
+        <v>15</v>
+      </c>
+      <c r="AC67" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G68" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="H68" s="45"/>
+      <c r="I68" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="J68" s="45"/>
+      <c r="K68" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="L68" s="50"/>
+      <c r="P68" s="35">
+        <v>7</v>
+      </c>
+      <c r="Q68" s="26">
+        <v>11</v>
+      </c>
+      <c r="R68" s="3">
+        <v>15</v>
+      </c>
+      <c r="S68" s="4">
+        <v>3</v>
+      </c>
+      <c r="U68" s="35">
+        <v>7</v>
+      </c>
+      <c r="V68" s="26">
+        <v>2</v>
+      </c>
+      <c r="W68" s="3">
+        <v>1</v>
+      </c>
+      <c r="X68" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z68" s="35">
+        <v>7</v>
+      </c>
+      <c r="AA68" s="26">
+        <v>5</v>
+      </c>
+      <c r="AB68" s="3">
+        <v>12</v>
+      </c>
+      <c r="AC68" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="G69" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="H69" s="38">
+        <f>AVERAGE(Q86:Q95)</f>
+        <v>16.2</v>
+      </c>
+      <c r="I69" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J69" s="38">
+        <f>AVERAGE(V86:V95)</f>
+        <v>23.6</v>
+      </c>
+      <c r="K69" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="L69" s="39">
+        <f>AVERAGE(AA74:AA83)</f>
+        <v>11.6</v>
+      </c>
+      <c r="P69" s="35">
+        <v>8</v>
+      </c>
+      <c r="Q69" s="26">
+        <v>9</v>
+      </c>
+      <c r="R69" s="3">
+        <v>4</v>
+      </c>
+      <c r="S69" s="4">
+        <v>2</v>
+      </c>
+      <c r="U69" s="35">
+        <v>8</v>
+      </c>
+      <c r="V69" s="26">
+        <v>3</v>
+      </c>
+      <c r="W69" s="3">
+        <v>11</v>
+      </c>
+      <c r="X69" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z69" s="35">
+        <v>8</v>
+      </c>
+      <c r="AA69" s="26">
+        <v>16</v>
+      </c>
+      <c r="AB69" s="3">
+        <v>38</v>
+      </c>
+      <c r="AC69" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="G70" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H70" s="1">
+        <f>AVERAGE(Q62:Q71)</f>
+        <v>11.2</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J70" s="1">
+        <f>AVERAGE(V62:V71)</f>
+        <v>7.6</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L70" s="41">
+        <f>AVERAGE(AA62:AA71)</f>
+        <v>10.3</v>
+      </c>
+      <c r="P70" s="35">
+        <v>9</v>
+      </c>
+      <c r="Q70" s="26">
+        <v>13</v>
+      </c>
+      <c r="R70" s="3">
+        <v>16</v>
+      </c>
+      <c r="S70" s="4">
+        <v>3</v>
+      </c>
+      <c r="U70" s="35">
+        <v>9</v>
+      </c>
+      <c r="V70" s="26">
+        <v>17</v>
+      </c>
+      <c r="W70" s="3">
+        <v>38</v>
+      </c>
+      <c r="X70" s="4">
+        <v>2</v>
+      </c>
+      <c r="Z70" s="35">
+        <v>9</v>
+      </c>
+      <c r="AA70" s="26">
+        <v>5</v>
+      </c>
+      <c r="AB70" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC70" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G71" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="H71" s="43">
+        <f>AVERAGE(Q74:Q83)</f>
+        <v>4.7</v>
+      </c>
+      <c r="I71" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="J71" s="43">
+        <f>AVERAGE(V74:V83)</f>
+        <v>3.1</v>
+      </c>
+      <c r="K71" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="L71" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="P71" s="36">
+        <v>10</v>
+      </c>
+      <c r="Q71" s="27">
+        <v>28</v>
+      </c>
+      <c r="R71" s="5">
+        <v>37</v>
+      </c>
+      <c r="S71" s="6">
+        <v>8</v>
+      </c>
+      <c r="U71" s="36">
+        <v>10</v>
+      </c>
+      <c r="V71" s="27">
+        <v>5</v>
+      </c>
+      <c r="W71" s="5">
+        <v>22</v>
+      </c>
+      <c r="X71" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z71" s="36">
+        <v>10</v>
+      </c>
+      <c r="AA71" s="27">
+        <v>3</v>
+      </c>
+      <c r="AB71" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC71" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P72" t="s">
+        <v>4</v>
+      </c>
+      <c r="U72" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z72" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="7:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P73" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q73" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="R73" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="S73" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="U73" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="V73" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="W73" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="X73" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z73" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA73" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB73" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC73" s="33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="P74" s="34">
+        <v>1</v>
+      </c>
+      <c r="Q74" s="7">
+        <v>4</v>
+      </c>
+      <c r="R74" s="28">
+        <v>12</v>
+      </c>
+      <c r="S74" s="29">
+        <v>2</v>
+      </c>
+      <c r="U74" s="34">
+        <v>1</v>
+      </c>
+      <c r="V74" s="7">
+        <v>1</v>
+      </c>
+      <c r="W74" s="28">
+        <v>0</v>
+      </c>
+      <c r="X74" s="29">
+        <v>1</v>
+      </c>
+      <c r="Z74" s="34">
+        <v>1</v>
+      </c>
+      <c r="AA74" s="7">
+        <v>12</v>
+      </c>
+      <c r="AB74" s="28">
+        <v>6</v>
+      </c>
+      <c r="AC74" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="P75" s="35">
+        <v>2</v>
+      </c>
+      <c r="Q75" s="26">
+        <v>5</v>
+      </c>
+      <c r="R75" s="3">
+        <v>22</v>
+      </c>
+      <c r="S75" s="4">
+        <v>2</v>
+      </c>
+      <c r="U75" s="35">
+        <v>2</v>
+      </c>
+      <c r="V75" s="26">
+        <v>2</v>
+      </c>
+      <c r="W75" s="3">
+        <v>21</v>
+      </c>
+      <c r="X75" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z75" s="35">
+        <v>2</v>
+      </c>
+      <c r="AA75" s="26">
+        <v>17</v>
+      </c>
+      <c r="AB75" s="3">
+        <v>18</v>
+      </c>
+      <c r="AC75" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="P76" s="35">
+        <v>3</v>
+      </c>
+      <c r="Q76" s="26">
+        <v>3</v>
+      </c>
+      <c r="R76" s="3">
+        <v>11</v>
+      </c>
+      <c r="S76" s="4">
+        <v>1</v>
+      </c>
+      <c r="U76" s="35">
+        <v>3</v>
+      </c>
+      <c r="V76" s="26">
+        <v>1</v>
+      </c>
+      <c r="W76" s="3">
+        <v>0</v>
+      </c>
+      <c r="X76" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z76" s="35">
+        <v>3</v>
+      </c>
+      <c r="AA76" s="26">
+        <v>3</v>
+      </c>
+      <c r="AB76" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC76" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="P77" s="35">
+        <v>4</v>
+      </c>
+      <c r="Q77" s="26">
+        <v>4</v>
+      </c>
+      <c r="R77" s="3">
+        <v>12</v>
+      </c>
+      <c r="S77" s="4">
+        <v>2</v>
+      </c>
+      <c r="U77" s="35">
+        <v>4</v>
+      </c>
+      <c r="V77" s="26">
+        <v>8</v>
+      </c>
+      <c r="W77" s="3">
+        <v>14</v>
+      </c>
+      <c r="X77" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z77" s="35">
+        <v>4</v>
+      </c>
+      <c r="AA77" s="26">
+        <v>6</v>
+      </c>
+      <c r="AB77" s="3">
+        <v>3</v>
+      </c>
+      <c r="AC77" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="P78" s="35">
+        <v>5</v>
+      </c>
+      <c r="Q78" s="26">
+        <v>3</v>
+      </c>
+      <c r="R78" s="3">
+        <v>1</v>
+      </c>
+      <c r="S78" s="4">
+        <v>1</v>
+      </c>
+      <c r="U78" s="35">
+        <v>5</v>
+      </c>
+      <c r="V78" s="26">
+        <v>1</v>
+      </c>
+      <c r="W78" s="3">
+        <v>0</v>
+      </c>
+      <c r="X78" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z78" s="35">
+        <v>5</v>
+      </c>
+      <c r="AA78" s="26">
+        <v>4</v>
+      </c>
+      <c r="AB78" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC78" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="P79" s="35">
+        <v>6</v>
+      </c>
+      <c r="Q79" s="26">
+        <v>2</v>
+      </c>
+      <c r="R79" s="3">
+        <v>11</v>
+      </c>
+      <c r="S79" s="4">
+        <v>1</v>
+      </c>
+      <c r="U79" s="35">
+        <v>6</v>
+      </c>
+      <c r="V79" s="26">
+        <v>4</v>
+      </c>
+      <c r="W79" s="3">
+        <v>2</v>
+      </c>
+      <c r="X79" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z79" s="35">
+        <v>6</v>
+      </c>
+      <c r="AA79" s="26">
+        <v>10</v>
+      </c>
+      <c r="AB79" s="3">
+        <v>5</v>
+      </c>
+      <c r="AC79" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="7:29" x14ac:dyDescent="0.35">
+      <c r="P80" s="35">
+        <v>7</v>
+      </c>
+      <c r="Q80" s="26">
+        <v>6</v>
+      </c>
+      <c r="R80" s="3">
+        <v>3</v>
+      </c>
+      <c r="S80" s="4">
+        <v>2</v>
+      </c>
+      <c r="U80" s="35">
+        <v>7</v>
+      </c>
+      <c r="V80" s="26">
+        <v>7</v>
+      </c>
+      <c r="W80" s="3">
+        <v>13</v>
+      </c>
+      <c r="X80" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z80" s="35">
+        <v>7</v>
+      </c>
+      <c r="AA80" s="26">
+        <v>9</v>
+      </c>
+      <c r="AB80" s="3">
+        <v>14</v>
+      </c>
+      <c r="AC80" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="16:29" x14ac:dyDescent="0.35">
+      <c r="P81" s="35">
+        <v>8</v>
+      </c>
+      <c r="Q81" s="26">
+        <v>5</v>
+      </c>
+      <c r="R81" s="3">
+        <v>12</v>
+      </c>
+      <c r="S81" s="4">
+        <v>1</v>
+      </c>
+      <c r="U81" s="35">
+        <v>8</v>
+      </c>
+      <c r="V81" s="26">
+        <v>2</v>
+      </c>
+      <c r="W81" s="3">
+        <v>1</v>
+      </c>
+      <c r="X81" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z81" s="35">
+        <v>8</v>
+      </c>
+      <c r="AA81" s="26">
+        <v>14</v>
+      </c>
+      <c r="AB81" s="3">
+        <v>7</v>
+      </c>
+      <c r="AC81" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="16:29" x14ac:dyDescent="0.35">
+      <c r="P82" s="35">
+        <v>9</v>
+      </c>
+      <c r="Q82" s="26">
+        <v>9</v>
+      </c>
+      <c r="R82" s="3">
+        <v>14</v>
+      </c>
+      <c r="S82" s="4">
+        <v>2</v>
+      </c>
+      <c r="U82" s="35">
+        <v>9</v>
+      </c>
+      <c r="V82" s="26">
+        <v>2</v>
+      </c>
+      <c r="W82" s="3">
+        <v>1</v>
+      </c>
+      <c r="X82" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z82" s="35">
+        <v>9</v>
+      </c>
+      <c r="AA82" s="26">
+        <v>34</v>
+      </c>
+      <c r="AB82" s="3">
+        <v>27</v>
+      </c>
+      <c r="AC82" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="16:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P83" s="36">
+        <v>10</v>
+      </c>
+      <c r="Q83" s="27">
+        <v>6</v>
+      </c>
+      <c r="R83" s="5">
+        <v>3</v>
+      </c>
+      <c r="S83" s="6">
+        <v>2</v>
+      </c>
+      <c r="U83" s="36">
+        <v>10</v>
+      </c>
+      <c r="V83" s="27">
+        <v>3</v>
+      </c>
+      <c r="W83" s="5">
+        <v>11</v>
+      </c>
+      <c r="X83" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z83" s="36">
+        <v>10</v>
+      </c>
+      <c r="AA83" s="27">
+        <v>7</v>
+      </c>
+      <c r="AB83" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC83" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="16:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P84" t="s">
+        <v>10</v>
+      </c>
+      <c r="U84" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z84" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="16:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P85" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q85" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="R85" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="S85" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="U85" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="V85" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="W85" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="X85" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z85" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA85" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB85" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC85" s="33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="16:29" x14ac:dyDescent="0.35">
+      <c r="P86" s="34">
+        <v>1</v>
+      </c>
+      <c r="Q86" s="7">
+        <v>3</v>
+      </c>
+      <c r="R86" s="28">
+        <v>1</v>
+      </c>
+      <c r="S86" s="29">
+        <v>1</v>
+      </c>
+      <c r="U86" s="34">
+        <v>1</v>
+      </c>
+      <c r="V86" s="7">
+        <v>35</v>
+      </c>
+      <c r="W86" s="28">
+        <v>17</v>
+      </c>
+      <c r="X86" s="29">
+        <v>5</v>
+      </c>
+      <c r="Z86" s="34">
+        <v>1</v>
+      </c>
+      <c r="AA86" s="7"/>
+      <c r="AB86" s="28"/>
+      <c r="AC86" s="29"/>
+    </row>
+    <row r="87" spans="16:29" x14ac:dyDescent="0.35">
+      <c r="P87" s="35">
+        <v>2</v>
+      </c>
+      <c r="Q87" s="26">
+        <v>12</v>
+      </c>
+      <c r="R87" s="3">
+        <v>24</v>
+      </c>
+      <c r="S87" s="4">
+        <v>3</v>
+      </c>
+      <c r="U87" s="35">
+        <v>2</v>
+      </c>
+      <c r="V87" s="26">
+        <v>50</v>
+      </c>
+      <c r="W87" s="3">
+        <v>65</v>
+      </c>
+      <c r="X87" s="4">
+        <v>6</v>
+      </c>
+      <c r="Z87" s="35">
+        <v>2</v>
+      </c>
+      <c r="AA87" s="26"/>
+      <c r="AB87" s="3"/>
+      <c r="AC87" s="4"/>
+    </row>
+    <row r="88" spans="16:29" x14ac:dyDescent="0.35">
+      <c r="P88" s="35">
+        <v>3</v>
+      </c>
+      <c r="Q88" s="26">
+        <v>34</v>
+      </c>
+      <c r="R88" s="3">
+        <v>17</v>
+      </c>
+      <c r="S88" s="4">
+        <v>6</v>
+      </c>
+      <c r="U88" s="35">
+        <v>3</v>
+      </c>
+      <c r="V88" s="26">
+        <v>8</v>
+      </c>
+      <c r="W88" s="3">
+        <v>4</v>
+      </c>
+      <c r="X88" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z88" s="35">
+        <v>3</v>
+      </c>
+      <c r="AA88" s="26"/>
+      <c r="AB88" s="3"/>
+      <c r="AC88" s="4"/>
+    </row>
+    <row r="89" spans="16:29" x14ac:dyDescent="0.35">
+      <c r="P89" s="35">
+        <v>4</v>
+      </c>
+      <c r="Q89" s="26">
+        <v>19</v>
+      </c>
+      <c r="R89" s="3">
+        <v>9</v>
+      </c>
+      <c r="S89" s="4">
+        <v>4</v>
+      </c>
+      <c r="U89" s="35">
+        <v>4</v>
+      </c>
+      <c r="V89" s="26">
+        <v>7</v>
+      </c>
+      <c r="W89" s="3">
+        <v>23</v>
+      </c>
+      <c r="X89" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z89" s="35">
+        <v>4</v>
+      </c>
+      <c r="AA89" s="26"/>
+      <c r="AB89" s="3"/>
+      <c r="AC89" s="4"/>
+    </row>
+    <row r="90" spans="16:29" x14ac:dyDescent="0.35">
+      <c r="P90" s="35">
+        <v>5</v>
+      </c>
+      <c r="Q90" s="26">
+        <v>30</v>
+      </c>
+      <c r="R90" s="3">
+        <v>15</v>
+      </c>
+      <c r="S90" s="4">
+        <v>5</v>
+      </c>
+      <c r="U90" s="35">
+        <v>5</v>
+      </c>
+      <c r="V90" s="26">
+        <v>9</v>
+      </c>
+      <c r="W90" s="3">
+        <v>14</v>
+      </c>
+      <c r="X90" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z90" s="35">
+        <v>5</v>
+      </c>
+      <c r="AA90" s="26"/>
+      <c r="AB90" s="3"/>
+      <c r="AC90" s="4"/>
+    </row>
+    <row r="91" spans="16:29" x14ac:dyDescent="0.35">
+      <c r="P91" s="35">
+        <v>6</v>
+      </c>
+      <c r="Q91" s="26">
+        <v>21</v>
+      </c>
+      <c r="R91" s="3">
+        <v>11</v>
+      </c>
+      <c r="S91" s="4">
+        <v>4</v>
+      </c>
+      <c r="U91" s="35">
+        <v>6</v>
+      </c>
+      <c r="V91" s="26">
+        <v>52</v>
+      </c>
+      <c r="W91" s="3">
+        <v>46</v>
+      </c>
+      <c r="X91" s="4">
+        <v>6</v>
+      </c>
+      <c r="Z91" s="35">
+        <v>6</v>
+      </c>
+      <c r="AA91" s="26"/>
+      <c r="AB91" s="3"/>
+      <c r="AC91" s="4"/>
+    </row>
+    <row r="92" spans="16:29" x14ac:dyDescent="0.35">
+      <c r="P92" s="35">
+        <v>7</v>
+      </c>
+      <c r="Q92" s="26">
+        <v>10</v>
+      </c>
+      <c r="R92" s="3">
+        <v>18</v>
+      </c>
+      <c r="S92" s="4">
+        <v>2</v>
+      </c>
+      <c r="U92" s="35">
+        <v>7</v>
+      </c>
+      <c r="V92" s="26">
+        <v>49</v>
+      </c>
+      <c r="W92" s="3">
+        <v>44</v>
+      </c>
+      <c r="X92" s="4">
+        <v>5</v>
+      </c>
+      <c r="Z92" s="35">
+        <v>7</v>
+      </c>
+      <c r="AA92" s="26"/>
+      <c r="AB92" s="3"/>
+      <c r="AC92" s="4"/>
+    </row>
+    <row r="93" spans="16:29" x14ac:dyDescent="0.35">
+      <c r="P93" s="35">
+        <v>8</v>
+      </c>
+      <c r="Q93" s="26">
+        <v>6</v>
+      </c>
+      <c r="R93" s="3">
+        <v>3</v>
+      </c>
+      <c r="S93" s="4">
+        <v>1</v>
+      </c>
+      <c r="U93" s="35">
+        <v>8</v>
+      </c>
+      <c r="V93" s="26">
+        <v>11</v>
+      </c>
+      <c r="W93" s="3">
+        <v>15</v>
+      </c>
+      <c r="X93" s="4">
+        <v>2</v>
+      </c>
+      <c r="Z93" s="35">
+        <v>8</v>
+      </c>
+      <c r="AA93" s="26"/>
+      <c r="AB93" s="3"/>
+      <c r="AC93" s="4"/>
+    </row>
+    <row r="94" spans="16:29" x14ac:dyDescent="0.35">
+      <c r="P94" s="35">
+        <v>9</v>
+      </c>
+      <c r="Q94" s="26">
+        <v>15</v>
+      </c>
+      <c r="R94" s="3">
+        <v>17</v>
+      </c>
+      <c r="S94" s="4">
+        <v>6</v>
+      </c>
+      <c r="U94" s="35">
+        <v>9</v>
+      </c>
+      <c r="V94" s="26">
+        <v>12</v>
+      </c>
+      <c r="W94" s="3">
+        <v>6</v>
+      </c>
+      <c r="X94" s="4">
+        <v>2</v>
+      </c>
+      <c r="Z94" s="35">
+        <v>9</v>
+      </c>
+      <c r="AA94" s="26"/>
+      <c r="AB94" s="3"/>
+      <c r="AC94" s="4"/>
+    </row>
+    <row r="95" spans="16:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P95" s="36">
+        <v>10</v>
+      </c>
+      <c r="Q95" s="27">
+        <v>12</v>
+      </c>
+      <c r="R95" s="5">
+        <v>22</v>
+      </c>
+      <c r="S95" s="6">
+        <v>3</v>
+      </c>
+      <c r="U95" s="36">
+        <v>10</v>
+      </c>
+      <c r="V95" s="27">
+        <v>3</v>
+      </c>
+      <c r="W95" s="5">
+        <v>1</v>
+      </c>
+      <c r="X95" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z95" s="36">
+        <v>10</v>
+      </c>
+      <c r="AA95" s="27"/>
+      <c r="AB95" s="5"/>
+      <c r="AC95" s="6"/>
+    </row>
   </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="G34:L34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="G40:L40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="G61:L61"/>
+    <mergeCell ref="G67:L67"/>
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="I62:J62"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="K68:L68"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>